<commit_message>
update sicilia 7 apr
</commit_message>
<xml_diff>
--- a/sicilia/covid19-sicilia-timeseries.xlsx
+++ b/sicilia/covid19-sicilia-timeseries.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="18">
   <si>
     <t>provincia</t>
   </si>
@@ -830,11 +830,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T118"/>
+  <dimension ref="A1:T127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1385,49 +1385,38 @@
     </row>
     <row r="15" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
-        <v>43915</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>9</v>
+        <v>43928</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
       </c>
       <c r="C15" s="12">
-        <v>262458</v>
-      </c>
-      <c r="D15" s="9">
-        <v>43</v>
-      </c>
-      <c r="E15" s="9">
-        <v>0</v>
-      </c>
-      <c r="F15" s="9">
-        <v>0</v>
-      </c>
-      <c r="G15" s="9">
-        <v>0</v>
-      </c>
-      <c r="H15" s="9">
+        <v>434870</v>
+      </c>
+      <c r="D15" s="5">
+        <v>107</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>2</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
         <f>SUM(D15+F15+G15)</f>
-        <v>43</v>
-      </c>
-      <c r="I15" s="9">
+        <v>110</v>
+      </c>
+      <c r="I15" s="5">
         <f>H15-E15-F15-G15</f>
-        <v>43</v>
-      </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
+        <v>107</v>
+      </c>
     </row>
     <row r="16" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
-        <v>43916</v>
+        <v>43915</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>9</v>
@@ -1436,10 +1425,10 @@
         <v>262458</v>
       </c>
       <c r="D16" s="9">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E16" s="9">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F16" s="9">
         <v>0</v>
@@ -1449,23 +1438,27 @@
       </c>
       <c r="H16" s="9">
         <f>SUM(D16+F16+G16)</f>
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I16" s="9">
         <f>H16-E16-F16-G16</f>
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="J16" s="13"/>
       <c r="K16" s="14"/>
       <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
     </row>
     <row r="17" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
-        <v>43917</v>
+        <v>43916</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>9</v>
@@ -1474,24 +1467,24 @@
         <v>262458</v>
       </c>
       <c r="D17" s="9">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="9">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F17" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G17" s="9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H17" s="9">
         <f>SUM(D17+F17+G17)</f>
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="I17" s="9">
         <f>H17-E17-F17-G17</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="14"/>
@@ -1503,7 +1496,7 @@
     </row>
     <row r="18" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
-        <v>43918</v>
+        <v>43917</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>9</v>
@@ -1512,24 +1505,24 @@
         <v>262458</v>
       </c>
       <c r="D18" s="9">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" s="9">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F18" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G18" s="9">
         <v>4</v>
       </c>
       <c r="H18" s="9">
         <f>SUM(D18+F18+G18)</f>
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I18" s="9">
         <f>H18-E18-F18-G18</f>
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="14"/>
@@ -1541,7 +1534,7 @@
     </row>
     <row r="19" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
-        <v>43919</v>
+        <v>43918</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>9</v>
@@ -1550,7 +1543,7 @@
         <v>262458</v>
       </c>
       <c r="D19" s="9">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E19" s="9">
         <v>19</v>
@@ -1563,11 +1556,11 @@
       </c>
       <c r="H19" s="9">
         <f>SUM(D19+F19+G19)</f>
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="I19" s="9">
         <f>H19-E19-F19-G19</f>
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="J19" s="13"/>
       <c r="K19" s="14"/>
@@ -1579,7 +1572,7 @@
     </row>
     <row r="20" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
-        <v>43920</v>
+        <v>43919</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>9</v>
@@ -1588,7 +1581,7 @@
         <v>262458</v>
       </c>
       <c r="D20" s="9">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E20" s="9">
         <v>19</v>
@@ -1601,11 +1594,11 @@
       </c>
       <c r="H20" s="9">
         <f>SUM(D20+F20+G20)</f>
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I20" s="9">
         <f>H20-E20-F20-G20</f>
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J20" s="13"/>
       <c r="K20" s="14"/>
@@ -1617,7 +1610,7 @@
     </row>
     <row r="21" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
-        <v>43921</v>
+        <v>43920</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>9</v>
@@ -1626,13 +1619,13 @@
         <v>262458</v>
       </c>
       <c r="D21" s="9">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E21" s="9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F21" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G21" s="9">
         <v>4</v>
@@ -1655,7 +1648,7 @@
     </row>
     <row r="22" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="11">
-        <v>43922</v>
+        <v>43921</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>9</v>
@@ -1664,7 +1657,7 @@
         <v>262458</v>
       </c>
       <c r="D22" s="9">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E22" s="9">
         <v>18</v>
@@ -1673,15 +1666,15 @@
         <v>4</v>
       </c>
       <c r="G22" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H22" s="9">
         <f>SUM(D22+F22+G22)</f>
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I22" s="9">
         <f>H22-E22-F22-G22</f>
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="J22" s="13"/>
       <c r="K22" s="14"/>
@@ -1691,9 +1684,9 @@
       <c r="O22" s="14"/>
       <c r="P22" s="14"/>
     </row>
-    <row r="23" spans="1:20" ht="18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="11">
-        <v>43923</v>
+        <v>43922</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>9</v>
@@ -1702,10 +1695,10 @@
         <v>262458</v>
       </c>
       <c r="D23" s="9">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E23" s="9">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F23" s="9">
         <v>4</v>
@@ -1715,13 +1708,13 @@
       </c>
       <c r="H23" s="9">
         <f>SUM(D23+F23+G23)</f>
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="I23" s="9">
         <f>H23-E23-F23-G23</f>
-        <v>51</v>
-      </c>
-      <c r="J23" s="16"/>
+        <v>49</v>
+      </c>
+      <c r="J23" s="13"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
       <c r="M23" s="14"/>
@@ -1731,7 +1724,7 @@
     </row>
     <row r="24" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A24" s="11">
-        <v>43924</v>
+        <v>43923</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>9</v>
@@ -1740,7 +1733,7 @@
         <v>262458</v>
       </c>
       <c r="D24" s="9">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E24" s="9">
         <v>20</v>
@@ -1749,15 +1742,15 @@
         <v>4</v>
       </c>
       <c r="G24" s="9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H24" s="9">
         <f>SUM(D24+F24+G24)</f>
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I24" s="9">
         <f>H24-E24-F24-G24</f>
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J24" s="16"/>
       <c r="K24" s="14"/>
@@ -1767,9 +1760,9 @@
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
     </row>
-    <row r="25" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A25" s="11">
-        <v>43925</v>
+        <v>43924</v>
       </c>
       <c r="B25" s="8" t="s">
         <v>9</v>
@@ -1778,26 +1771,26 @@
         <v>262458</v>
       </c>
       <c r="D25" s="9">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E25" s="9">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F25" s="9">
         <v>4</v>
       </c>
       <c r="G25" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H25" s="9">
         <f>SUM(D25+F25+G25)</f>
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="I25" s="9">
         <f>H25-E25-F25-G25</f>
-        <v>57</v>
-      </c>
-      <c r="J25" s="13"/>
+        <v>53</v>
+      </c>
+      <c r="J25" s="16"/>
       <c r="K25" s="14"/>
       <c r="L25" s="14"/>
       <c r="M25" s="14"/>
@@ -1807,7 +1800,7 @@
     </row>
     <row r="26" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
-        <v>43926</v>
+        <v>43925</v>
       </c>
       <c r="B26" s="8" t="s">
         <v>9</v>
@@ -1816,10 +1809,10 @@
         <v>262458</v>
       </c>
       <c r="D26" s="9">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E26" s="9">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F26" s="9">
         <v>4</v>
@@ -1829,11 +1822,11 @@
       </c>
       <c r="H26" s="9">
         <f>SUM(D26+F26+G26)</f>
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="I26" s="9">
         <f>H26-E26-F26-G26</f>
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="J26" s="13"/>
       <c r="K26" s="14"/>
@@ -1845,7 +1838,7 @@
     </row>
     <row r="27" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
-        <v>43927</v>
+        <v>43926</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>9</v>
@@ -1854,24 +1847,24 @@
         <v>262458</v>
       </c>
       <c r="D27" s="9">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E27" s="9">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F27" s="9">
         <v>4</v>
       </c>
       <c r="G27" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H27" s="9">
         <f>SUM(D27+F27+G27)</f>
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I27" s="9">
         <f>H27-E27-F27-G27</f>
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J27" s="13"/>
       <c r="K27" s="14"/>
@@ -1883,87 +1876,76 @@
     </row>
     <row r="28" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="11">
-        <v>43915</v>
+        <v>43927</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C28" s="12">
-        <v>1107702</v>
+        <v>262458</v>
       </c>
       <c r="D28" s="9">
-        <v>288</v>
+        <v>92</v>
       </c>
       <c r="E28" s="9">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F28" s="9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G28" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H28" s="9">
         <f>SUM(D28+F28+G28)</f>
-        <v>288</v>
+        <v>104</v>
       </c>
       <c r="I28" s="9">
         <f>H28-E28-F28-G28</f>
-        <v>288</v>
+        <v>70</v>
       </c>
       <c r="J28" s="13"/>
       <c r="K28" s="14"/>
       <c r="L28" s="14"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
     </row>
     <row r="29" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="11">
-        <v>43916</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>10</v>
+        <v>43928</v>
+      </c>
+      <c r="B29" t="s">
+        <v>9</v>
       </c>
       <c r="C29" s="12">
-        <v>1107702</v>
-      </c>
-      <c r="D29" s="9">
-        <v>321</v>
-      </c>
-      <c r="E29" s="9">
-        <v>132</v>
-      </c>
-      <c r="F29" s="9">
-        <v>0</v>
-      </c>
-      <c r="G29" s="9">
-        <v>0</v>
-      </c>
-      <c r="H29" s="9">
+        <v>262458</v>
+      </c>
+      <c r="D29" s="5">
+        <v>93</v>
+      </c>
+      <c r="E29" s="5">
+        <v>22</v>
+      </c>
+      <c r="F29" s="5">
+        <v>4</v>
+      </c>
+      <c r="G29" s="5">
+        <v>8</v>
+      </c>
+      <c r="H29" s="5">
         <f>SUM(D29+F29+G29)</f>
-        <v>321</v>
-      </c>
-      <c r="I29" s="9">
+        <v>105</v>
+      </c>
+      <c r="I29" s="5">
         <f>H29-E29-F29-G29</f>
-        <v>189</v>
-      </c>
-      <c r="J29" s="13"/>
-      <c r="K29" s="14"/>
-      <c r="L29" s="14"/>
-      <c r="M29" s="14"/>
-      <c r="N29" s="14"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
+        <v>71</v>
+      </c>
     </row>
     <row r="30" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="11">
-        <v>43917</v>
+        <v>43915</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>10</v>
@@ -1972,36 +1954,40 @@
         <v>1107702</v>
       </c>
       <c r="D30" s="9">
-        <v>344</v>
+        <v>288</v>
       </c>
       <c r="E30" s="9">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="F30" s="9">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G30" s="9">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="H30" s="9">
         <f>SUM(D30+F30+G30)</f>
-        <v>375</v>
+        <v>288</v>
       </c>
       <c r="I30" s="9">
         <f>H30-E30-F30-G30</f>
-        <v>215</v>
+        <v>288</v>
       </c>
       <c r="J30" s="13"/>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
-      <c r="M30" s="14"/>
-      <c r="N30" s="14"/>
-      <c r="O30" s="14"/>
-      <c r="P30" s="14"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="15"/>
     </row>
     <row r="31" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="11">
-        <v>43918</v>
+        <v>43916</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>10</v>
@@ -2010,24 +1996,24 @@
         <v>1107702</v>
       </c>
       <c r="D31" s="9">
-        <v>350</v>
+        <v>321</v>
       </c>
       <c r="E31" s="9">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="F31" s="9">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G31" s="9">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="H31" s="9">
         <f>SUM(D31+F31+G31)</f>
-        <v>387</v>
+        <v>321</v>
       </c>
       <c r="I31" s="9">
         <f>H31-E31-F31-G31</f>
-        <v>223</v>
+        <v>189</v>
       </c>
       <c r="J31" s="13"/>
       <c r="K31" s="14"/>
@@ -2039,7 +2025,7 @@
     </row>
     <row r="32" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="11">
-        <v>43919</v>
+        <v>43917</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>10</v>
@@ -2048,24 +2034,24 @@
         <v>1107702</v>
       </c>
       <c r="D32" s="9">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="E32" s="9">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F32" s="9">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G32" s="9">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H32" s="9">
         <f>SUM(D32+F32+G32)</f>
-        <v>407</v>
+        <v>375</v>
       </c>
       <c r="I32" s="9">
         <f>H32-E32-F32-G32</f>
-        <v>232</v>
+        <v>215</v>
       </c>
       <c r="J32" s="13"/>
       <c r="K32" s="14"/>
@@ -2077,7 +2063,7 @@
     </row>
     <row r="33" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="11">
-        <v>43920</v>
+        <v>43918</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>10</v>
@@ -2086,24 +2072,24 @@
         <v>1107702</v>
       </c>
       <c r="D33" s="9">
-        <v>405</v>
+        <v>350</v>
       </c>
       <c r="E33" s="9">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="F33" s="9">
         <v>16</v>
       </c>
       <c r="G33" s="9">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H33" s="9">
         <f>SUM(D33+F33+G33)</f>
-        <v>448</v>
+        <v>387</v>
       </c>
       <c r="I33" s="9">
         <f>H33-E33-F33-G33</f>
-        <v>263</v>
+        <v>223</v>
       </c>
       <c r="J33" s="13"/>
       <c r="K33" s="14"/>
@@ -2115,7 +2101,7 @@
     </row>
     <row r="34" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
-        <v>43921</v>
+        <v>43919</v>
       </c>
       <c r="B34" s="8" t="s">
         <v>10</v>
@@ -2124,24 +2110,24 @@
         <v>1107702</v>
       </c>
       <c r="D34" s="9">
-        <v>453</v>
+        <v>368</v>
       </c>
       <c r="E34" s="9">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="F34" s="9">
         <v>16</v>
       </c>
       <c r="G34" s="9">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H34" s="9">
         <f>SUM(D34+F34+G34)</f>
-        <v>498</v>
+        <v>407</v>
       </c>
       <c r="I34" s="9">
         <f>H34-E34-F34-G34</f>
-        <v>303</v>
+        <v>232</v>
       </c>
       <c r="J34" s="13"/>
       <c r="K34" s="14"/>
@@ -2153,7 +2139,7 @@
     </row>
     <row r="35" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="11">
-        <v>43922</v>
+        <v>43920</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>10</v>
@@ -2162,24 +2148,24 @@
         <v>1107702</v>
       </c>
       <c r="D35" s="9">
-        <v>456</v>
+        <v>405</v>
       </c>
       <c r="E35" s="9">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="F35" s="9">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G35" s="9">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H35" s="9">
         <f>SUM(D35+F35+G35)</f>
-        <v>510</v>
+        <v>448</v>
       </c>
       <c r="I35" s="9">
         <f>H35-E35-F35-G35</f>
-        <v>303</v>
+        <v>263</v>
       </c>
       <c r="J35" s="13"/>
       <c r="K35" s="14"/>
@@ -2191,7 +2177,7 @@
     </row>
     <row r="36" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="11">
-        <v>43923</v>
+        <v>43921</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>10</v>
@@ -2200,24 +2186,24 @@
         <v>1107702</v>
       </c>
       <c r="D36" s="9">
-        <v>486</v>
+        <v>453</v>
       </c>
       <c r="E36" s="9">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F36" s="9">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G36" s="9">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H36" s="9">
         <f>SUM(D36+F36+G36)</f>
-        <v>544</v>
+        <v>498</v>
       </c>
       <c r="I36" s="9">
         <f>H36-E36-F36-G36</f>
-        <v>332</v>
+        <v>303</v>
       </c>
       <c r="J36" s="13"/>
       <c r="K36" s="14"/>
@@ -2227,9 +2213,9 @@
       <c r="O36" s="14"/>
       <c r="P36" s="14"/>
     </row>
-    <row r="37" spans="1:20" ht="18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
-        <v>43924</v>
+        <v>43922</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>10</v>
@@ -2238,26 +2224,26 @@
         <v>1107702</v>
       </c>
       <c r="D37" s="9">
-        <v>500</v>
+        <v>456</v>
       </c>
       <c r="E37" s="9">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="F37" s="9">
         <v>21</v>
       </c>
       <c r="G37" s="9">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="H37" s="9">
         <f>SUM(D37+F37+G37)</f>
-        <v>559</v>
+        <v>510</v>
       </c>
       <c r="I37" s="9">
         <f>H37-E37-F37-G37</f>
-        <v>326</v>
-      </c>
-      <c r="J37" s="16"/>
+        <v>303</v>
+      </c>
+      <c r="J37" s="13"/>
       <c r="K37" s="14"/>
       <c r="L37" s="14"/>
       <c r="M37" s="14"/>
@@ -2267,7 +2253,7 @@
     </row>
     <row r="38" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="11">
-        <v>43925</v>
+        <v>43923</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>10</v>
@@ -2276,24 +2262,24 @@
         <v>1107702</v>
       </c>
       <c r="D38" s="9">
-        <v>506</v>
+        <v>486</v>
       </c>
       <c r="E38" s="9">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F38" s="9">
         <v>21</v>
       </c>
       <c r="G38" s="9">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H38" s="9">
         <f>SUM(D38+F38+G38)</f>
-        <v>569</v>
+        <v>544</v>
       </c>
       <c r="I38" s="9">
         <f>H38-E38-F38-G38</f>
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="J38" s="13"/>
       <c r="K38" s="14"/>
@@ -2303,9 +2289,9 @@
       <c r="O38" s="14"/>
       <c r="P38" s="14"/>
     </row>
-    <row r="39" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
-        <v>43926</v>
+        <v>43924</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>10</v>
@@ -2314,26 +2300,26 @@
         <v>1107702</v>
       </c>
       <c r="D39" s="9">
-        <v>525</v>
+        <v>500</v>
       </c>
       <c r="E39" s="9">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="F39" s="9">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G39" s="9">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H39" s="9">
         <f>SUM(D39+F39+G39)</f>
-        <v>594</v>
+        <v>559</v>
       </c>
       <c r="I39" s="9">
         <f>H39-E39-F39-G39</f>
-        <v>372</v>
-      </c>
-      <c r="J39" s="13"/>
+        <v>326</v>
+      </c>
+      <c r="J39" s="16"/>
       <c r="K39" s="14"/>
       <c r="L39" s="14"/>
       <c r="M39" s="14"/>
@@ -2343,7 +2329,7 @@
     </row>
     <row r="40" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="11">
-        <v>43927</v>
+        <v>43925</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>10</v>
@@ -2352,24 +2338,24 @@
         <v>1107702</v>
       </c>
       <c r="D40" s="9">
-        <v>540</v>
+        <v>506</v>
       </c>
       <c r="E40" s="9">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F40" s="9">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G40" s="9">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H40" s="9">
         <f>SUM(D40+F40+G40)</f>
-        <v>614</v>
+        <v>569</v>
       </c>
       <c r="I40" s="9">
         <f>H40-E40-F40-G40</f>
-        <v>381</v>
+        <v>348</v>
       </c>
       <c r="J40" s="13"/>
       <c r="K40" s="14"/>
@@ -2381,75 +2367,71 @@
     </row>
     <row r="41" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="11">
-        <v>43915</v>
+        <v>43926</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C41" s="12">
-        <v>164788</v>
+        <v>1107702</v>
       </c>
       <c r="D41" s="9">
-        <v>83</v>
+        <v>525</v>
       </c>
       <c r="E41" s="9">
-        <v>0</v>
+        <v>153</v>
       </c>
       <c r="F41" s="9">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G41" s="9">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="H41" s="9">
         <f>SUM(D41+F41+G41)</f>
-        <v>83</v>
+        <v>594</v>
       </c>
       <c r="I41" s="9">
         <f>H41-E41-F41-G41</f>
-        <v>83</v>
+        <v>372</v>
       </c>
       <c r="J41" s="13"/>
       <c r="K41" s="14"/>
       <c r="L41" s="14"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
-      <c r="T41" s="15"/>
+      <c r="M41" s="14"/>
+      <c r="N41" s="14"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="14"/>
     </row>
     <row r="42" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="11">
-        <v>43916</v>
+        <v>43927</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C42" s="12">
-        <v>164788</v>
+        <v>1107702</v>
       </c>
       <c r="D42" s="9">
-        <v>126</v>
+        <v>540</v>
       </c>
       <c r="E42" s="9">
-        <v>55</v>
+        <v>159</v>
       </c>
       <c r="F42" s="9">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G42" s="9">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="H42" s="9">
         <f>SUM(D42+F42+G42)</f>
-        <v>126</v>
+        <v>614</v>
       </c>
       <c r="I42" s="9">
         <f>H42-E42-F42-G42</f>
-        <v>71</v>
+        <v>381</v>
       </c>
       <c r="J42" s="13"/>
       <c r="K42" s="14"/>
@@ -2461,45 +2443,38 @@
     </row>
     <row r="43" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="11">
-        <v>43917</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>11</v>
+        <v>43928</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
       </c>
       <c r="C43" s="12">
-        <v>164788</v>
-      </c>
-      <c r="D43" s="9">
-        <v>147</v>
-      </c>
-      <c r="E43" s="9">
-        <v>89</v>
-      </c>
-      <c r="F43" s="9">
-        <v>1</v>
-      </c>
-      <c r="G43" s="9">
-        <v>7</v>
-      </c>
-      <c r="H43" s="9">
+        <v>1107702</v>
+      </c>
+      <c r="D43" s="5">
+        <v>551</v>
+      </c>
+      <c r="E43" s="5">
+        <v>155</v>
+      </c>
+      <c r="F43" s="5">
+        <v>28</v>
+      </c>
+      <c r="G43" s="5">
+        <v>51</v>
+      </c>
+      <c r="H43" s="5">
         <f>SUM(D43+F43+G43)</f>
-        <v>155</v>
-      </c>
-      <c r="I43" s="9">
+        <v>630</v>
+      </c>
+      <c r="I43" s="5">
         <f>H43-E43-F43-G43</f>
-        <v>58</v>
-      </c>
-      <c r="J43" s="13"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
+        <v>396</v>
+      </c>
     </row>
     <row r="44" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="11">
-        <v>43918</v>
+        <v>43915</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>11</v>
@@ -2508,36 +2483,40 @@
         <v>164788</v>
       </c>
       <c r="D44" s="9">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="E44" s="9">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="F44" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G44" s="9">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H44" s="9">
         <f>SUM(D44+F44+G44)</f>
-        <v>168</v>
+        <v>83</v>
       </c>
       <c r="I44" s="9">
         <f>H44-E44-F44-G44</f>
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="J44" s="13"/>
       <c r="K44" s="14"/>
       <c r="L44" s="14"/>
-      <c r="M44" s="14"/>
-      <c r="N44" s="14"/>
-      <c r="O44" s="14"/>
-      <c r="P44" s="14"/>
+      <c r="M44" s="15"/>
+      <c r="N44" s="12"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="15"/>
+      <c r="R44" s="15"/>
+      <c r="S44" s="15"/>
+      <c r="T44" s="15"/>
     </row>
     <row r="45" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="11">
-        <v>43919</v>
+        <v>43916</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>11</v>
@@ -2546,24 +2525,24 @@
         <v>164788</v>
       </c>
       <c r="D45" s="9">
-        <v>181</v>
+        <v>126</v>
       </c>
       <c r="E45" s="9">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="F45" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G45" s="9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H45" s="9">
         <f>SUM(D45+F45+G45)</f>
-        <v>192</v>
+        <v>126</v>
       </c>
       <c r="I45" s="9">
         <f>H45-E45-F45-G45</f>
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="J45" s="13"/>
       <c r="K45" s="14"/>
@@ -2575,7 +2554,7 @@
     </row>
     <row r="46" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="11">
-        <v>43920</v>
+        <v>43917</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>11</v>
@@ -2584,24 +2563,24 @@
         <v>164788</v>
       </c>
       <c r="D46" s="9">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="E46" s="9">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="F46" s="9">
         <v>1</v>
       </c>
       <c r="G46" s="9">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="H46" s="9">
         <f>SUM(D46+F46+G46)</f>
-        <v>195</v>
+        <v>155</v>
       </c>
       <c r="I46" s="9">
         <f>H46-E46-F46-G46</f>
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J46" s="13"/>
       <c r="K46" s="14"/>
@@ -2613,7 +2592,7 @@
     </row>
     <row r="47" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="11">
-        <v>43921</v>
+        <v>43918</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>11</v>
@@ -2622,24 +2601,24 @@
         <v>164788</v>
       </c>
       <c r="D47" s="9">
-        <v>191</v>
+        <v>158</v>
       </c>
       <c r="E47" s="9">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="F47" s="9">
         <v>1</v>
       </c>
       <c r="G47" s="9">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H47" s="9">
         <f>SUM(D47+F47+G47)</f>
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="I47" s="9">
         <f>H47-E47-F47-G47</f>
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J47" s="13"/>
       <c r="K47" s="14"/>
@@ -2651,7 +2630,7 @@
     </row>
     <row r="48" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="11">
-        <v>43922</v>
+        <v>43919</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>11</v>
@@ -2660,20 +2639,20 @@
         <v>164788</v>
       </c>
       <c r="D48" s="9">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="E48" s="9">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="F48" s="9">
         <v>1</v>
       </c>
       <c r="G48" s="9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H48" s="9">
         <f>SUM(D48+F48+G48)</f>
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="I48" s="9">
         <f>H48-E48-F48-G48</f>
@@ -2689,7 +2668,7 @@
     </row>
     <row r="49" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="11">
-        <v>43923</v>
+        <v>43920</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>11</v>
@@ -2698,10 +2677,10 @@
         <v>164788</v>
       </c>
       <c r="D49" s="9">
-        <v>226</v>
+        <v>183</v>
       </c>
       <c r="E49" s="9">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="F49" s="9">
         <v>1</v>
@@ -2711,11 +2690,11 @@
       </c>
       <c r="H49" s="9">
         <f>SUM(D49+F49+G49)</f>
-        <v>238</v>
+        <v>195</v>
       </c>
       <c r="I49" s="9">
         <f>H49-E49-F49-G49</f>
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="J49" s="13"/>
       <c r="K49" s="14"/>
@@ -2725,9 +2704,9 @@
       <c r="O49" s="14"/>
       <c r="P49" s="14"/>
     </row>
-    <row r="50" spans="1:20" ht="18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="11">
-        <v>43924</v>
+        <v>43921</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>11</v>
@@ -2736,10 +2715,10 @@
         <v>164788</v>
       </c>
       <c r="D50" s="9">
-        <v>245</v>
+        <v>191</v>
       </c>
       <c r="E50" s="9">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="F50" s="9">
         <v>1</v>
@@ -2749,13 +2728,13 @@
       </c>
       <c r="H50" s="9">
         <f>SUM(D50+F50+G50)</f>
-        <v>257</v>
+        <v>203</v>
       </c>
       <c r="I50" s="9">
         <f>H50-E50-F50-G50</f>
-        <v>106</v>
-      </c>
-      <c r="J50" s="16"/>
+        <v>71</v>
+      </c>
+      <c r="J50" s="13"/>
       <c r="K50" s="14"/>
       <c r="L50" s="14"/>
       <c r="M50" s="14"/>
@@ -2765,7 +2744,7 @@
     </row>
     <row r="51" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="11">
-        <v>43925</v>
+        <v>43922</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>11</v>
@@ -2774,24 +2753,24 @@
         <v>164788</v>
       </c>
       <c r="D51" s="9">
-        <v>266</v>
+        <v>212</v>
       </c>
       <c r="E51" s="9">
-        <v>162</v>
+        <v>123</v>
       </c>
       <c r="F51" s="9">
         <v>1</v>
       </c>
       <c r="G51" s="9">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H51" s="9">
         <f>SUM(D51+F51+G51)</f>
-        <v>280</v>
+        <v>224</v>
       </c>
       <c r="I51" s="9">
         <f>H51-E51-F51-G51</f>
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="J51" s="13"/>
       <c r="K51" s="14"/>
@@ -2803,7 +2782,7 @@
     </row>
     <row r="52" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="11">
-        <v>43926</v>
+        <v>43923</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>11</v>
@@ -2812,24 +2791,24 @@
         <v>164788</v>
       </c>
       <c r="D52" s="9">
-        <v>270</v>
+        <v>226</v>
       </c>
       <c r="E52" s="9">
-        <v>170</v>
+        <v>133</v>
       </c>
       <c r="F52" s="9">
         <v>1</v>
       </c>
       <c r="G52" s="9">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H52" s="9">
         <f>SUM(D52+F52+G52)</f>
-        <v>284</v>
+        <v>238</v>
       </c>
       <c r="I52" s="9">
         <f>H52-E52-F52-G52</f>
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J52" s="13"/>
       <c r="K52" s="14"/>
@@ -2839,9 +2818,9 @@
       <c r="O52" s="14"/>
       <c r="P52" s="14"/>
     </row>
-    <row r="53" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" ht="18" x14ac:dyDescent="0.3">
       <c r="A53" s="11">
-        <v>43927</v>
+        <v>43924</v>
       </c>
       <c r="B53" s="8" t="s">
         <v>11</v>
@@ -2850,26 +2829,26 @@
         <v>164788</v>
       </c>
       <c r="D53" s="9">
-        <v>271</v>
+        <v>245</v>
       </c>
       <c r="E53" s="9">
-        <v>168</v>
+        <v>139</v>
       </c>
       <c r="F53" s="9">
         <v>1</v>
       </c>
       <c r="G53" s="9">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H53" s="9">
         <f>SUM(D53+F53+G53)</f>
-        <v>287</v>
+        <v>257</v>
       </c>
       <c r="I53" s="9">
         <f>H53-E53-F53-G53</f>
-        <v>103</v>
-      </c>
-      <c r="J53" s="13"/>
+        <v>106</v>
+      </c>
+      <c r="J53" s="16"/>
       <c r="K53" s="14"/>
       <c r="L53" s="14"/>
       <c r="M53" s="14"/>
@@ -2879,75 +2858,71 @@
     </row>
     <row r="54" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="11">
-        <v>43915</v>
+        <v>43925</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C54" s="12">
-        <v>626876</v>
+        <v>164788</v>
       </c>
       <c r="D54" s="9">
-        <v>168</v>
+        <v>266</v>
       </c>
       <c r="E54" s="9">
-        <v>0</v>
+        <v>162</v>
       </c>
       <c r="F54" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54" s="9">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H54" s="9">
         <f>SUM(D54+F54+G54)</f>
-        <v>168</v>
+        <v>280</v>
       </c>
       <c r="I54" s="9">
         <f>H54-E54-F54-G54</f>
-        <v>168</v>
+        <v>104</v>
       </c>
       <c r="J54" s="13"/>
       <c r="K54" s="14"/>
       <c r="L54" s="14"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="12"/>
-      <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="15"/>
-      <c r="R54" s="15"/>
-      <c r="S54" s="15"/>
-      <c r="T54" s="15"/>
+      <c r="M54" s="14"/>
+      <c r="N54" s="14"/>
+      <c r="O54" s="14"/>
+      <c r="P54" s="14"/>
     </row>
     <row r="55" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="11">
-        <v>43916</v>
+        <v>43926</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C55" s="12">
-        <v>626876</v>
+        <v>164788</v>
       </c>
       <c r="D55" s="9">
-        <v>212</v>
+        <v>270</v>
       </c>
       <c r="E55" s="9">
-        <v>94</v>
+        <v>170</v>
       </c>
       <c r="F55" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55" s="9">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H55" s="9">
         <f>SUM(D55+F55+G55)</f>
-        <v>212</v>
+        <v>284</v>
       </c>
       <c r="I55" s="9">
         <f>H55-E55-F55-G55</f>
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="J55" s="13"/>
       <c r="K55" s="14"/>
@@ -2959,33 +2934,33 @@
     </row>
     <row r="56" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="11">
-        <v>43917</v>
+        <v>43927</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C56" s="12">
-        <v>626876</v>
+        <v>164788</v>
       </c>
       <c r="D56" s="9">
-        <v>216</v>
+        <v>271</v>
       </c>
       <c r="E56" s="9">
-        <v>126</v>
+        <v>168</v>
       </c>
       <c r="F56" s="9">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G56" s="9">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H56" s="9">
         <f>SUM(D56+F56+G56)</f>
-        <v>227</v>
+        <v>287</v>
       </c>
       <c r="I56" s="9">
         <f>H56-E56-F56-G56</f>
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="J56" s="13"/>
       <c r="K56" s="14"/>
@@ -2997,45 +2972,38 @@
     </row>
     <row r="57" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="11">
-        <v>43918</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>12</v>
+        <v>43928</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
       </c>
       <c r="C57" s="12">
-        <v>626876</v>
-      </c>
-      <c r="D57" s="9">
-        <v>262</v>
-      </c>
-      <c r="E57" s="9">
-        <v>133</v>
-      </c>
-      <c r="F57" s="9">
-        <v>3</v>
-      </c>
-      <c r="G57" s="9">
-        <v>14</v>
-      </c>
-      <c r="H57" s="9">
+        <v>164788</v>
+      </c>
+      <c r="D57" s="5">
+        <v>273</v>
+      </c>
+      <c r="E57" s="5">
+        <v>168</v>
+      </c>
+      <c r="F57" s="5">
+        <v>1</v>
+      </c>
+      <c r="G57" s="5">
+        <v>15</v>
+      </c>
+      <c r="H57" s="5">
         <f>SUM(D57+F57+G57)</f>
-        <v>279</v>
-      </c>
-      <c r="I57" s="9">
+        <v>289</v>
+      </c>
+      <c r="I57" s="5">
         <f>H57-E57-F57-G57</f>
-        <v>129</v>
-      </c>
-      <c r="J57" s="13"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
-      <c r="O57" s="14"/>
-      <c r="P57" s="14"/>
+        <v>105</v>
+      </c>
     </row>
     <row r="58" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="11">
-        <v>43919</v>
+        <v>43915</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>12</v>
@@ -3044,36 +3012,40 @@
         <v>626876</v>
       </c>
       <c r="D58" s="9">
-        <v>266</v>
+        <v>168</v>
       </c>
       <c r="E58" s="9">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="F58" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G58" s="9">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="H58" s="9">
         <f>SUM(D58+F58+G58)</f>
-        <v>289</v>
+        <v>168</v>
       </c>
       <c r="I58" s="9">
         <f>H58-E58-F58-G58</f>
-        <v>137</v>
+        <v>168</v>
       </c>
       <c r="J58" s="13"/>
       <c r="K58" s="14"/>
       <c r="L58" s="14"/>
-      <c r="M58" s="14"/>
-      <c r="N58" s="14"/>
-      <c r="O58" s="14"/>
-      <c r="P58" s="14"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="12"/>
+      <c r="O58" s="15"/>
+      <c r="P58" s="15"/>
+      <c r="Q58" s="15"/>
+      <c r="R58" s="15"/>
+      <c r="S58" s="15"/>
+      <c r="T58" s="15"/>
     </row>
     <row r="59" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="11">
-        <v>43920</v>
+        <v>43916</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>12</v>
@@ -3082,24 +3054,24 @@
         <v>626876</v>
       </c>
       <c r="D59" s="9">
-        <v>280</v>
+        <v>212</v>
       </c>
       <c r="E59" s="9">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="F59" s="9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G59" s="9">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H59" s="9">
         <f>SUM(D59+F59+G59)</f>
-        <v>305</v>
+        <v>212</v>
       </c>
       <c r="I59" s="9">
         <f>H59-E59-F59-G59</f>
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="J59" s="13"/>
       <c r="K59" s="14"/>
@@ -3111,7 +3083,7 @@
     </row>
     <row r="60" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="11">
-        <v>43921</v>
+        <v>43917</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>12</v>
@@ -3120,24 +3092,24 @@
         <v>626876</v>
       </c>
       <c r="D60" s="9">
-        <v>283</v>
+        <v>216</v>
       </c>
       <c r="E60" s="9">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F60" s="9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G60" s="9">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H60" s="9">
         <f>SUM(D60+F60+G60)</f>
-        <v>311</v>
+        <v>227</v>
       </c>
       <c r="I60" s="9">
         <f>H60-E60-F60-G60</f>
-        <v>155</v>
+        <v>90</v>
       </c>
       <c r="J60" s="13"/>
       <c r="K60" s="14"/>
@@ -3149,7 +3121,7 @@
     </row>
     <row r="61" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="11">
-        <v>43922</v>
+        <v>43918</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>12</v>
@@ -3158,24 +3130,24 @@
         <v>626876</v>
       </c>
       <c r="D61" s="9">
-        <v>288</v>
+        <v>262</v>
       </c>
       <c r="E61" s="9">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F61" s="9">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G61" s="9">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H61" s="9">
         <f>SUM(D61+F61+G61)</f>
-        <v>319</v>
+        <v>279</v>
       </c>
       <c r="I61" s="9">
         <f>H61-E61-F61-G61</f>
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="J61" s="13"/>
       <c r="K61" s="14"/>
@@ -3187,7 +3159,7 @@
     </row>
     <row r="62" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="11">
-        <v>43923</v>
+        <v>43919</v>
       </c>
       <c r="B62" s="8" t="s">
         <v>12</v>
@@ -3196,24 +3168,24 @@
         <v>626876</v>
       </c>
       <c r="D62" s="9">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="E62" s="9">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="F62" s="9">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G62" s="9">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H62" s="9">
         <f>SUM(D62+F62+G62)</f>
-        <v>323</v>
+        <v>289</v>
       </c>
       <c r="I62" s="9">
         <f>H62-E62-F62-G62</f>
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="J62" s="13"/>
       <c r="K62" s="14"/>
@@ -3225,7 +3197,7 @@
     </row>
     <row r="63" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="11">
-        <v>43924</v>
+        <v>43920</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>12</v>
@@ -3234,24 +3206,24 @@
         <v>626876</v>
       </c>
       <c r="D63" s="9">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="E63" s="9">
         <v>128</v>
       </c>
       <c r="F63" s="9">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G63" s="9">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H63" s="9">
         <f>SUM(D63+F63+G63)</f>
-        <v>337</v>
+        <v>305</v>
       </c>
       <c r="I63" s="9">
         <f>H63-E63-F63-G63</f>
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="J63" s="13"/>
       <c r="K63" s="14"/>
@@ -3263,7 +3235,7 @@
     </row>
     <row r="64" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="11">
-        <v>43925</v>
+        <v>43921</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>12</v>
@@ -3272,24 +3244,24 @@
         <v>626876</v>
       </c>
       <c r="D64" s="9">
-        <v>306</v>
+        <v>283</v>
       </c>
       <c r="E64" s="9">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F64" s="9">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G64" s="9">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H64" s="9">
         <f>SUM(D64+F64+G64)</f>
-        <v>344</v>
+        <v>311</v>
       </c>
       <c r="I64" s="9">
         <f>H64-E64-F64-G64</f>
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="J64" s="13"/>
       <c r="K64" s="14"/>
@@ -3301,7 +3273,7 @@
     </row>
     <row r="65" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="11">
-        <v>43926</v>
+        <v>43922</v>
       </c>
       <c r="B65" s="8" t="s">
         <v>12</v>
@@ -3310,24 +3282,24 @@
         <v>626876</v>
       </c>
       <c r="D65" s="9">
-        <v>314</v>
+        <v>288</v>
       </c>
       <c r="E65" s="9">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="F65" s="9">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G65" s="9">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H65" s="9">
         <f>SUM(D65+F65+G65)</f>
-        <v>353</v>
+        <v>319</v>
       </c>
       <c r="I65" s="9">
         <f>H65-E65-F65-G65</f>
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="J65" s="13"/>
       <c r="K65" s="14"/>
@@ -3339,7 +3311,7 @@
     </row>
     <row r="66" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="11">
-        <v>43927</v>
+        <v>43923</v>
       </c>
       <c r="B66" s="8" t="s">
         <v>12</v>
@@ -3348,24 +3320,24 @@
         <v>626876</v>
       </c>
       <c r="D66" s="9">
-        <v>320</v>
+        <v>289</v>
       </c>
       <c r="E66" s="9">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="F66" s="9">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G66" s="9">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H66" s="9">
         <f>SUM(D66+F66+G66)</f>
-        <v>362</v>
+        <v>323</v>
       </c>
       <c r="I66" s="9">
         <f>H66-E66-F66-G66</f>
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="J66" s="13"/>
       <c r="K66" s="14"/>
@@ -3377,75 +3349,71 @@
     </row>
     <row r="67" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="11">
-        <v>43915</v>
+        <v>43924</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C67" s="12">
-        <v>1252588</v>
+        <v>626876</v>
       </c>
       <c r="D67" s="9">
-        <v>186</v>
+        <v>300</v>
       </c>
       <c r="E67" s="9">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="F67" s="9">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G67" s="9">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H67" s="9">
         <f>SUM(D67+F67+G67)</f>
-        <v>186</v>
+        <v>337</v>
       </c>
       <c r="I67" s="9">
         <f>H67-E67-F67-G67</f>
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="J67" s="13"/>
       <c r="K67" s="14"/>
       <c r="L67" s="14"/>
-      <c r="M67" s="15"/>
-      <c r="N67" s="12"/>
-      <c r="O67" s="12"/>
-      <c r="P67" s="15"/>
-      <c r="Q67" s="15"/>
-      <c r="R67" s="15"/>
-      <c r="S67" s="15"/>
-      <c r="T67" s="15"/>
+      <c r="M67" s="14"/>
+      <c r="N67" s="14"/>
+      <c r="O67" s="14"/>
+      <c r="P67" s="14"/>
     </row>
     <row r="68" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="11">
-        <v>43916</v>
+        <v>43925</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C68" s="12">
-        <v>1252588</v>
+        <v>626876</v>
       </c>
       <c r="D68" s="9">
-        <v>197</v>
+        <v>306</v>
       </c>
       <c r="E68" s="9">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="F68" s="9">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G68" s="9">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="H68" s="9">
         <f>SUM(D68+F68+G68)</f>
-        <v>197</v>
+        <v>344</v>
       </c>
       <c r="I68" s="9">
         <f>H68-E68-F68-G68</f>
-        <v>141</v>
+        <v>176</v>
       </c>
       <c r="J68" s="13"/>
       <c r="K68" s="14"/>
@@ -3457,33 +3425,33 @@
     </row>
     <row r="69" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="11">
-        <v>43917</v>
+        <v>43926</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C69" s="12">
-        <v>1252588</v>
+        <v>626876</v>
       </c>
       <c r="D69" s="9">
-        <v>204</v>
+        <v>314</v>
       </c>
       <c r="E69" s="9">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="F69" s="9">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G69" s="9">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="H69" s="9">
         <f>SUM(D69+F69+G69)</f>
-        <v>219</v>
+        <v>353</v>
       </c>
       <c r="I69" s="9">
         <f>H69-E69-F69-G69</f>
-        <v>122</v>
+        <v>176</v>
       </c>
       <c r="J69" s="13"/>
       <c r="K69" s="14"/>
@@ -3495,33 +3463,33 @@
     </row>
     <row r="70" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="11">
-        <v>43918</v>
+        <v>43927</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C70" s="12">
-        <v>1252588</v>
+        <v>626876</v>
       </c>
       <c r="D70" s="9">
-        <v>213</v>
+        <v>320</v>
       </c>
       <c r="E70" s="9">
-        <v>80</v>
+        <v>139</v>
       </c>
       <c r="F70" s="9">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G70" s="9">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="H70" s="9">
         <f>SUM(D70+F70+G70)</f>
-        <v>232</v>
+        <v>362</v>
       </c>
       <c r="I70" s="9">
         <f>H70-E70-F70-G70</f>
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="J70" s="13"/>
       <c r="K70" s="14"/>
@@ -3533,45 +3501,38 @@
     </row>
     <row r="71" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="11">
-        <v>43919</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>13</v>
+        <v>43928</v>
+      </c>
+      <c r="B71" t="s">
+        <v>12</v>
       </c>
       <c r="C71" s="12">
-        <v>1252588</v>
-      </c>
-      <c r="D71" s="9">
-        <v>216</v>
-      </c>
-      <c r="E71" s="9">
-        <v>78</v>
-      </c>
-      <c r="F71" s="9">
-        <v>14</v>
-      </c>
-      <c r="G71" s="9">
-        <v>6</v>
-      </c>
-      <c r="H71" s="9">
+        <v>626876</v>
+      </c>
+      <c r="D71" s="5">
+        <v>327</v>
+      </c>
+      <c r="E71" s="5">
+        <v>145</v>
+      </c>
+      <c r="F71" s="5">
+        <v>18</v>
+      </c>
+      <c r="G71" s="5">
+        <v>25</v>
+      </c>
+      <c r="H71" s="5">
         <f>SUM(D71+F71+G71)</f>
-        <v>236</v>
-      </c>
-      <c r="I71" s="9">
+        <v>370</v>
+      </c>
+      <c r="I71" s="5">
         <f>H71-E71-F71-G71</f>
-        <v>138</v>
-      </c>
-      <c r="J71" s="13"/>
-      <c r="K71" s="14"/>
-      <c r="L71" s="14"/>
-      <c r="M71" s="14"/>
-      <c r="N71" s="14"/>
-      <c r="O71" s="14"/>
-      <c r="P71" s="14"/>
+        <v>182</v>
+      </c>
     </row>
     <row r="72" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="11">
-        <v>43920</v>
+        <v>43915</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>13</v>
@@ -3580,36 +3541,40 @@
         <v>1252588</v>
       </c>
       <c r="D72" s="9">
-        <v>229</v>
+        <v>186</v>
       </c>
       <c r="E72" s="9">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="F72" s="9">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G72" s="9">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="H72" s="9">
         <f>SUM(D72+F72+G72)</f>
-        <v>253</v>
+        <v>186</v>
       </c>
       <c r="I72" s="9">
         <f>H72-E72-F72-G72</f>
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="J72" s="13"/>
       <c r="K72" s="14"/>
       <c r="L72" s="14"/>
-      <c r="M72" s="14"/>
-      <c r="N72" s="14"/>
-      <c r="O72" s="14"/>
-      <c r="P72" s="14"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="12"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
+      <c r="S72" s="15"/>
+      <c r="T72" s="15"/>
     </row>
     <row r="73" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="11">
-        <v>43921</v>
+        <v>43916</v>
       </c>
       <c r="B73" s="8" t="s">
         <v>13</v>
@@ -3618,24 +3583,24 @@
         <v>1252588</v>
       </c>
       <c r="D73" s="9">
-        <v>236</v>
+        <v>197</v>
       </c>
       <c r="E73" s="9">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="F73" s="9">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="G73" s="9">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H73" s="9">
         <f>SUM(D73+F73+G73)</f>
-        <v>262</v>
+        <v>197</v>
       </c>
       <c r="I73" s="9">
         <f>H73-E73-F73-G73</f>
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="J73" s="13"/>
       <c r="K73" s="14"/>
@@ -3647,7 +3612,7 @@
     </row>
     <row r="74" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="11">
-        <v>43922</v>
+        <v>43917</v>
       </c>
       <c r="B74" s="8" t="s">
         <v>13</v>
@@ -3656,24 +3621,24 @@
         <v>1252588</v>
       </c>
       <c r="D74" s="9">
-        <v>245</v>
+        <v>204</v>
       </c>
       <c r="E74" s="9">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F74" s="9">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G74" s="9">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H74" s="9">
         <f>SUM(D74+F74+G74)</f>
-        <v>276</v>
+        <v>219</v>
       </c>
       <c r="I74" s="9">
         <f>H74-E74-F74-G74</f>
-        <v>166</v>
+        <v>122</v>
       </c>
       <c r="J74" s="13"/>
       <c r="K74" s="14"/>
@@ -3685,7 +3650,7 @@
     </row>
     <row r="75" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="11">
-        <v>43923</v>
+        <v>43918</v>
       </c>
       <c r="B75" s="8" t="s">
         <v>13</v>
@@ -3694,24 +3659,24 @@
         <v>1252588</v>
       </c>
       <c r="D75" s="9">
-        <v>250</v>
+        <v>213</v>
       </c>
       <c r="E75" s="9">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F75" s="9">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G75" s="9">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H75" s="9">
         <f>SUM(D75+F75+G75)</f>
-        <v>282</v>
+        <v>232</v>
       </c>
       <c r="I75" s="9">
         <f>H75-E75-F75-G75</f>
-        <v>172</v>
+        <v>133</v>
       </c>
       <c r="J75" s="13"/>
       <c r="K75" s="14"/>
@@ -3723,7 +3688,7 @@
     </row>
     <row r="76" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="11">
-        <v>43924</v>
+        <v>43919</v>
       </c>
       <c r="B76" s="8" t="s">
         <v>13</v>
@@ -3732,24 +3697,24 @@
         <v>1252588</v>
       </c>
       <c r="D76" s="9">
-        <v>255</v>
+        <v>216</v>
       </c>
       <c r="E76" s="9">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F76" s="9">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G76" s="9">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="H76" s="9">
         <f>SUM(D76+F76+G76)</f>
-        <v>290</v>
+        <v>236</v>
       </c>
       <c r="I76" s="9">
         <f>H76-E76-F76-G76</f>
-        <v>179</v>
+        <v>138</v>
       </c>
       <c r="J76" s="13"/>
       <c r="K76" s="14"/>
@@ -3761,7 +3726,7 @@
     </row>
     <row r="77" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="11">
-        <v>43925</v>
+        <v>43920</v>
       </c>
       <c r="B77" s="8" t="s">
         <v>13</v>
@@ -3770,24 +3735,24 @@
         <v>1252588</v>
       </c>
       <c r="D77" s="9">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="E77" s="9">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F77" s="9">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G77" s="9">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H77" s="9">
         <f>SUM(D77+F77+G77)</f>
-        <v>296</v>
+        <v>253</v>
       </c>
       <c r="I77" s="9">
         <f>H77-E77-F77-G77</f>
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="J77" s="13"/>
       <c r="K77" s="14"/>
@@ -3799,7 +3764,7 @@
     </row>
     <row r="78" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="11">
-        <v>43926</v>
+        <v>43921</v>
       </c>
       <c r="B78" s="8" t="s">
         <v>13</v>
@@ -3808,24 +3773,24 @@
         <v>1252588</v>
       </c>
       <c r="D78" s="9">
-        <v>258</v>
+        <v>236</v>
       </c>
       <c r="E78" s="9">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="F78" s="9">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="G78" s="9">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H78" s="9">
         <f>SUM(D78+F78+G78)</f>
-        <v>299</v>
+        <v>262</v>
       </c>
       <c r="I78" s="9">
         <f>H78-E78-F78-G78</f>
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="J78" s="13"/>
       <c r="K78" s="14"/>
@@ -3837,7 +3802,7 @@
     </row>
     <row r="79" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="11">
-        <v>43927</v>
+        <v>43922</v>
       </c>
       <c r="B79" s="8" t="s">
         <v>13</v>
@@ -3846,24 +3811,24 @@
         <v>1252588</v>
       </c>
       <c r="D79" s="9">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="E79" s="9">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="F79" s="9">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G79" s="9">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H79" s="9">
         <f>SUM(D79+F79+G79)</f>
-        <v>301</v>
+        <v>276</v>
       </c>
       <c r="I79" s="9">
         <f>H79-E79-F79-G79</f>
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="J79" s="13"/>
       <c r="K79" s="14"/>
@@ -3875,75 +3840,71 @@
     </row>
     <row r="80" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="11">
-        <v>43915</v>
+        <v>43923</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C80" s="12">
-        <v>320893</v>
+        <v>1252588</v>
       </c>
       <c r="D80" s="9">
-        <v>21</v>
+        <v>250</v>
       </c>
       <c r="E80" s="9">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="F80" s="9">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G80" s="9">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H80" s="9">
         <f>SUM(D80+F80+G80)</f>
-        <v>21</v>
+        <v>282</v>
       </c>
       <c r="I80" s="9">
         <f>H80-E80-F80-G80</f>
-        <v>21</v>
+        <v>172</v>
       </c>
       <c r="J80" s="13"/>
       <c r="K80" s="14"/>
       <c r="L80" s="14"/>
-      <c r="M80" s="15"/>
-      <c r="N80" s="12"/>
-      <c r="O80" s="15"/>
-      <c r="P80" s="15"/>
-      <c r="Q80" s="15"/>
-      <c r="R80" s="15"/>
-      <c r="S80" s="15"/>
-      <c r="T80" s="15"/>
+      <c r="M80" s="14"/>
+      <c r="N80" s="14"/>
+      <c r="O80" s="14"/>
+      <c r="P80" s="14"/>
     </row>
     <row r="81" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="11">
-        <v>43916</v>
+        <v>43924</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C81" s="12">
-        <v>320893</v>
+        <v>1252588</v>
       </c>
       <c r="D81" s="9">
-        <v>27</v>
+        <v>255</v>
       </c>
       <c r="E81" s="9">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="F81" s="9">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G81" s="9">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H81" s="9">
         <f>SUM(D81+F81+G81)</f>
-        <v>27</v>
+        <v>290</v>
       </c>
       <c r="I81" s="9">
         <f>H81-E81-F81-G81</f>
-        <v>19</v>
+        <v>179</v>
       </c>
       <c r="J81" s="13"/>
       <c r="K81" s="14"/>
@@ -3955,33 +3916,33 @@
     </row>
     <row r="82" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="11">
-        <v>43917</v>
+        <v>43925</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C82" s="12">
-        <v>320893</v>
+        <v>1252588</v>
       </c>
       <c r="D82" s="9">
-        <v>29</v>
+        <v>260</v>
       </c>
       <c r="E82" s="9">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="F82" s="9">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="G82" s="9">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H82" s="9">
         <f>SUM(D82+F82+G82)</f>
-        <v>32</v>
+        <v>296</v>
       </c>
       <c r="I82" s="9">
         <f>H82-E82-F82-G82</f>
-        <v>21</v>
+        <v>183</v>
       </c>
       <c r="J82" s="13"/>
       <c r="K82" s="14"/>
@@ -3993,33 +3954,33 @@
     </row>
     <row r="83" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="11">
-        <v>43918</v>
+        <v>43926</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C83" s="12">
-        <v>320893</v>
+        <v>1252588</v>
       </c>
       <c r="D83" s="9">
+        <v>258</v>
+      </c>
+      <c r="E83" s="9">
+        <v>73</v>
+      </c>
+      <c r="F83" s="9">
         <v>29</v>
       </c>
-      <c r="E83" s="9">
-        <v>9</v>
-      </c>
-      <c r="F83" s="9">
-        <v>3</v>
-      </c>
       <c r="G83" s="9">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H83" s="9">
         <f>SUM(D83+F83+G83)</f>
-        <v>32</v>
+        <v>299</v>
       </c>
       <c r="I83" s="9">
         <f>H83-E83-F83-G83</f>
-        <v>20</v>
+        <v>185</v>
       </c>
       <c r="J83" s="13"/>
       <c r="K83" s="14"/>
@@ -4031,33 +3992,33 @@
     </row>
     <row r="84" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="11">
-        <v>43919</v>
+        <v>43927</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C84" s="12">
-        <v>320893</v>
+        <v>1252588</v>
       </c>
       <c r="D84" s="9">
-        <v>27</v>
+        <v>260</v>
       </c>
       <c r="E84" s="9">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="F84" s="9">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="G84" s="9">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H84" s="9">
         <f>SUM(D84+F84+G84)</f>
-        <v>32</v>
+        <v>301</v>
       </c>
       <c r="I84" s="9">
         <f>H84-E84-F84-G84</f>
-        <v>20</v>
+        <v>186</v>
       </c>
       <c r="J84" s="13"/>
       <c r="K84" s="14"/>
@@ -4069,45 +4030,38 @@
     </row>
     <row r="85" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="11">
-        <v>43920</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>14</v>
+        <v>43928</v>
+      </c>
+      <c r="B85" t="s">
+        <v>13</v>
       </c>
       <c r="C85" s="12">
-        <v>320893</v>
-      </c>
-      <c r="D85" s="9">
-        <v>30</v>
-      </c>
-      <c r="E85" s="9">
-        <v>8</v>
-      </c>
-      <c r="F85" s="9">
-        <v>3</v>
-      </c>
-      <c r="G85" s="9">
-        <v>2</v>
-      </c>
-      <c r="H85" s="9">
+        <v>1252588</v>
+      </c>
+      <c r="D85" s="5">
+        <v>276</v>
+      </c>
+      <c r="E85" s="5">
+        <v>74</v>
+      </c>
+      <c r="F85" s="5">
+        <v>29</v>
+      </c>
+      <c r="G85" s="5">
+        <v>12</v>
+      </c>
+      <c r="H85" s="5">
         <f>SUM(D85+F85+G85)</f>
-        <v>35</v>
-      </c>
-      <c r="I85" s="9">
+        <v>317</v>
+      </c>
+      <c r="I85" s="5">
         <f>H85-E85-F85-G85</f>
-        <v>22</v>
-      </c>
-      <c r="J85" s="13"/>
-      <c r="K85" s="14"/>
-      <c r="L85" s="14"/>
-      <c r="M85" s="14"/>
-      <c r="N85" s="14"/>
-      <c r="O85" s="14"/>
-      <c r="P85" s="14"/>
+        <v>202</v>
+      </c>
     </row>
     <row r="86" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="11">
-        <v>43921</v>
+        <v>43915</v>
       </c>
       <c r="B86" s="8" t="s">
         <v>14</v>
@@ -4116,36 +4070,40 @@
         <v>320893</v>
       </c>
       <c r="D86" s="9">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="E86" s="9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F86" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G86" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H86" s="9">
         <f>SUM(D86+F86+G86)</f>
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="I86" s="9">
         <f>H86-E86-F86-G86</f>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="J86" s="13"/>
       <c r="K86" s="14"/>
       <c r="L86" s="14"/>
-      <c r="M86" s="14"/>
-      <c r="N86" s="14"/>
-      <c r="O86" s="14"/>
-      <c r="P86" s="14"/>
+      <c r="M86" s="15"/>
+      <c r="N86" s="12"/>
+      <c r="O86" s="15"/>
+      <c r="P86" s="15"/>
+      <c r="Q86" s="15"/>
+      <c r="R86" s="15"/>
+      <c r="S86" s="15"/>
+      <c r="T86" s="15"/>
     </row>
     <row r="87" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="11">
-        <v>43922</v>
+        <v>43916</v>
       </c>
       <c r="B87" s="8" t="s">
         <v>14</v>
@@ -4154,24 +4112,24 @@
         <v>320893</v>
       </c>
       <c r="D87" s="9">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E87" s="9">
         <v>8</v>
       </c>
       <c r="F87" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G87" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H87" s="9">
         <f>SUM(D87+F87+G87)</f>
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="I87" s="9">
         <f>H87-E87-F87-G87</f>
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="J87" s="13"/>
       <c r="K87" s="14"/>
@@ -4183,7 +4141,7 @@
     </row>
     <row r="88" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="11">
-        <v>43923</v>
+        <v>43917</v>
       </c>
       <c r="B88" s="8" t="s">
         <v>14</v>
@@ -4192,24 +4150,24 @@
         <v>320893</v>
       </c>
       <c r="D88" s="9">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E88" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F88" s="9">
         <v>3</v>
       </c>
       <c r="G88" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H88" s="9">
         <f>SUM(D88+F88+G88)</f>
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="I88" s="9">
         <f>H88-E88-F88-G88</f>
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="J88" s="13"/>
       <c r="K88" s="14"/>
@@ -4221,7 +4179,7 @@
     </row>
     <row r="89" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="11">
-        <v>43924</v>
+        <v>43918</v>
       </c>
       <c r="B89" s="8" t="s">
         <v>14</v>
@@ -4230,7 +4188,7 @@
         <v>320893</v>
       </c>
       <c r="D89" s="9">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="E89" s="9">
         <v>9</v>
@@ -4239,15 +4197,15 @@
         <v>3</v>
       </c>
       <c r="G89" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H89" s="9">
         <f>SUM(D89+F89+G89)</f>
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="I89" s="9">
         <f>H89-E89-F89-G89</f>
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="J89" s="13"/>
       <c r="K89" s="14"/>
@@ -4259,7 +4217,7 @@
     </row>
     <row r="90" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="11">
-        <v>43925</v>
+        <v>43919</v>
       </c>
       <c r="B90" s="8" t="s">
         <v>14</v>
@@ -4268,24 +4226,24 @@
         <v>320893</v>
       </c>
       <c r="D90" s="9">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E90" s="9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F90" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G90" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H90" s="9">
         <f>SUM(D90+F90+G90)</f>
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="I90" s="9">
         <f>H90-E90-F90-G90</f>
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="J90" s="13"/>
       <c r="K90" s="14"/>
@@ -4297,7 +4255,7 @@
     </row>
     <row r="91" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="11">
-        <v>43926</v>
+        <v>43920</v>
       </c>
       <c r="B91" s="8" t="s">
         <v>14</v>
@@ -4306,24 +4264,24 @@
         <v>320893</v>
       </c>
       <c r="D91" s="9">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="E91" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F91" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G91" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H91" s="9">
         <f>SUM(D91+F91+G91)</f>
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I91" s="9">
         <f>H91-E91-F91-G91</f>
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="J91" s="13"/>
       <c r="K91" s="14"/>
@@ -4335,7 +4293,7 @@
     </row>
     <row r="92" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="11">
-        <v>43927</v>
+        <v>43921</v>
       </c>
       <c r="B92" s="8" t="s">
         <v>14</v>
@@ -4344,24 +4302,24 @@
         <v>320893</v>
       </c>
       <c r="D92" s="9">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E92" s="9">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F92" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G92" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H92" s="9">
         <f>SUM(D92+F92+G92)</f>
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="I92" s="9">
         <f>H92-E92-F92-G92</f>
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="J92" s="13"/>
       <c r="K92" s="14"/>
@@ -4373,75 +4331,71 @@
     </row>
     <row r="93" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="11">
-        <v>43915</v>
+        <v>43922</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C93" s="12">
-        <v>399224</v>
+        <v>320893</v>
       </c>
       <c r="D93" s="9">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E93" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F93" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G93" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H93" s="9">
         <f>SUM(D93+F93+G93)</f>
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="I93" s="9">
         <f>H93-E93-F93-G93</f>
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="J93" s="13"/>
       <c r="K93" s="14"/>
       <c r="L93" s="14"/>
-      <c r="M93" s="15"/>
-      <c r="N93" s="12"/>
-      <c r="O93" s="15"/>
-      <c r="P93" s="15"/>
-      <c r="Q93" s="15"/>
-      <c r="R93" s="15"/>
-      <c r="S93" s="15"/>
-      <c r="T93" s="15"/>
+      <c r="M93" s="14"/>
+      <c r="N93" s="14"/>
+      <c r="O93" s="14"/>
+      <c r="P93" s="14"/>
     </row>
     <row r="94" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="11">
-        <v>43916</v>
+        <v>43923</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C94" s="12">
-        <v>399224</v>
+        <v>320893</v>
       </c>
       <c r="D94" s="9">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="E94" s="9">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="F94" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G94" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H94" s="9">
         <f>SUM(D94+F94+G94)</f>
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="I94" s="9">
         <f>H94-E94-F94-G94</f>
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="J94" s="13"/>
       <c r="K94" s="14"/>
@@ -4453,33 +4407,33 @@
     </row>
     <row r="95" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="11">
-        <v>43917</v>
+        <v>43924</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C95" s="12">
-        <v>399224</v>
+        <v>320893</v>
       </c>
       <c r="D95" s="9">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="E95" s="9">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F95" s="9">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G95" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H95" s="9">
         <f>SUM(D95+F95+G95)</f>
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="I95" s="9">
         <f>H95-E95-F95-G95</f>
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="J95" s="13"/>
       <c r="K95" s="14"/>
@@ -4491,33 +4445,33 @@
     </row>
     <row r="96" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="11">
-        <v>43918</v>
+        <v>43925</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C96" s="12">
-        <v>399224</v>
+        <v>320893</v>
       </c>
       <c r="D96" s="9">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="E96" s="9">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="F96" s="9">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G96" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H96" s="9">
         <f>SUM(D96+F96+G96)</f>
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="I96" s="9">
         <f>H96-E96-F96-G96</f>
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J96" s="13"/>
       <c r="K96" s="14"/>
@@ -4529,33 +4483,33 @@
     </row>
     <row r="97" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="11">
-        <v>43919</v>
+        <v>43926</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C97" s="12">
-        <v>399224</v>
+        <v>320893</v>
       </c>
       <c r="D97" s="9">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="E97" s="9">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="F97" s="9">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G97" s="9">
         <v>3</v>
       </c>
       <c r="H97" s="9">
         <f>SUM(D97+F97+G97)</f>
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="I97" s="9">
         <f>H97-E97-F97-G97</f>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J97" s="13"/>
       <c r="K97" s="14"/>
@@ -4567,33 +4521,33 @@
     </row>
     <row r="98" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="11">
-        <v>43920</v>
+        <v>43927</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C98" s="12">
-        <v>399224</v>
+        <v>320893</v>
       </c>
       <c r="D98" s="9">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E98" s="9">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F98" s="9">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="G98" s="9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H98" s="9">
         <f>SUM(D98+F98+G98)</f>
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="I98" s="9">
         <f>H98-E98-F98-G98</f>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="J98" s="13"/>
       <c r="K98" s="14"/>
@@ -4605,45 +4559,38 @@
     </row>
     <row r="99" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="11">
-        <v>43921</v>
-      </c>
-      <c r="B99" s="8" t="s">
-        <v>15</v>
+        <v>43928</v>
+      </c>
+      <c r="B99" t="s">
+        <v>14</v>
       </c>
       <c r="C99" s="12">
-        <v>399224</v>
-      </c>
-      <c r="D99" s="9">
-        <v>66</v>
-      </c>
-      <c r="E99" s="9">
-        <v>36</v>
-      </c>
-      <c r="F99" s="9">
-        <v>21</v>
-      </c>
-      <c r="G99" s="9">
-        <v>6</v>
-      </c>
-      <c r="H99" s="9">
+        <v>320893</v>
+      </c>
+      <c r="D99" s="5">
+        <v>47</v>
+      </c>
+      <c r="E99" s="5">
+        <v>7</v>
+      </c>
+      <c r="F99" s="5">
+        <v>4</v>
+      </c>
+      <c r="G99" s="5">
+        <v>3</v>
+      </c>
+      <c r="H99" s="5">
         <f>SUM(D99+F99+G99)</f>
-        <v>93</v>
-      </c>
-      <c r="I99" s="9">
+        <v>54</v>
+      </c>
+      <c r="I99" s="5">
         <f>H99-E99-F99-G99</f>
-        <v>30</v>
-      </c>
-      <c r="J99" s="13"/>
-      <c r="K99" s="14"/>
-      <c r="L99" s="14"/>
-      <c r="M99" s="14"/>
-      <c r="N99" s="14"/>
-      <c r="O99" s="14"/>
-      <c r="P99" s="14"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="100" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="11">
-        <v>43922</v>
+        <v>43915</v>
       </c>
       <c r="B100" s="8" t="s">
         <v>15</v>
@@ -4652,36 +4599,40 @@
         <v>399224</v>
       </c>
       <c r="D100" s="9">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="E100" s="9">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="F100" s="9">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G100" s="9">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H100" s="9">
         <f>SUM(D100+F100+G100)</f>
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="I100" s="9">
         <f>H100-E100-F100-G100</f>
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="J100" s="13"/>
       <c r="K100" s="14"/>
       <c r="L100" s="14"/>
-      <c r="M100" s="14"/>
-      <c r="N100" s="14"/>
-      <c r="O100" s="14"/>
-      <c r="P100" s="14"/>
+      <c r="M100" s="15"/>
+      <c r="N100" s="12"/>
+      <c r="O100" s="15"/>
+      <c r="P100" s="15"/>
+      <c r="Q100" s="15"/>
+      <c r="R100" s="15"/>
+      <c r="S100" s="15"/>
+      <c r="T100" s="15"/>
     </row>
     <row r="101" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="11">
-        <v>43923</v>
+        <v>43916</v>
       </c>
       <c r="B101" s="8" t="s">
         <v>15</v>
@@ -4690,24 +4641,24 @@
         <v>399224</v>
       </c>
       <c r="D101" s="9">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E101" s="9">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F101" s="9">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="G101" s="9">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H101" s="9">
         <f>SUM(D101+F101+G101)</f>
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="I101" s="9">
         <f>H101-E101-F101-G101</f>
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J101" s="13"/>
       <c r="K101" s="14"/>
@@ -4719,7 +4670,7 @@
     </row>
     <row r="102" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="11">
-        <v>43924</v>
+        <v>43917</v>
       </c>
       <c r="B102" s="8" t="s">
         <v>15</v>
@@ -4728,24 +4679,24 @@
         <v>399224</v>
       </c>
       <c r="D102" s="9">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="E102" s="9">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="F102" s="9">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="G102" s="9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H102" s="9">
         <f>SUM(D102+F102+G102)</f>
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="I102" s="9">
         <f>H102-E102-F102-G102</f>
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="J102" s="13"/>
       <c r="K102" s="14"/>
@@ -4757,7 +4708,7 @@
     </row>
     <row r="103" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="11">
-        <v>43925</v>
+        <v>43918</v>
       </c>
       <c r="B103" s="8" t="s">
         <v>15</v>
@@ -4766,24 +4717,24 @@
         <v>399224</v>
       </c>
       <c r="D103" s="9">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E103" s="9">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="F103" s="9">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="G103" s="9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H103" s="9">
         <f>SUM(D103+F103+G103)</f>
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="I103" s="9">
         <f>H103-E103-F103-G103</f>
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J103" s="13"/>
       <c r="K103" s="14"/>
@@ -4795,7 +4746,7 @@
     </row>
     <row r="104" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="11">
-        <v>43926</v>
+        <v>43919</v>
       </c>
       <c r="B104" s="8" t="s">
         <v>15</v>
@@ -4804,24 +4755,24 @@
         <v>399224</v>
       </c>
       <c r="D104" s="9">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="E104" s="9">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F104" s="9">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="G104" s="9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H104" s="9">
         <f>SUM(D104+F104+G104)</f>
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="I104" s="9">
         <f>H104-E104-F104-G104</f>
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J104" s="13"/>
       <c r="K104" s="14"/>
@@ -4833,7 +4784,7 @@
     </row>
     <row r="105" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="11">
-        <v>43927</v>
+        <v>43920</v>
       </c>
       <c r="B105" s="8" t="s">
         <v>15</v>
@@ -4842,24 +4793,24 @@
         <v>399224</v>
       </c>
       <c r="D105" s="9">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="E105" s="9">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F105" s="9">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G105" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H105" s="9">
         <f>SUM(D105+F105+G105)</f>
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="I105" s="9">
         <f>H105-E105-F105-G105</f>
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="J105" s="13"/>
       <c r="K105" s="14"/>
@@ -4871,75 +4822,71 @@
     </row>
     <row r="106" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="11">
-        <v>43915</v>
+        <v>43921</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C106" s="12">
-        <v>430492</v>
+        <v>399224</v>
       </c>
       <c r="D106" s="9">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="E106" s="9">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="F106" s="9">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="G106" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H106" s="9">
         <f>SUM(D106+F106+G106)</f>
-        <v>48</v>
+        <v>93</v>
       </c>
       <c r="I106" s="9">
         <f>H106-E106-F106-G106</f>
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="J106" s="13"/>
       <c r="K106" s="14"/>
       <c r="L106" s="14"/>
-      <c r="M106" s="15"/>
-      <c r="N106" s="12"/>
-      <c r="O106" s="15"/>
-      <c r="P106" s="15"/>
-      <c r="Q106" s="15"/>
-      <c r="R106" s="15"/>
-      <c r="S106" s="15"/>
-      <c r="T106" s="15"/>
+      <c r="M106" s="14"/>
+      <c r="N106" s="14"/>
+      <c r="O106" s="14"/>
+      <c r="P106" s="14"/>
     </row>
     <row r="107" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="11">
-        <v>43916</v>
+        <v>43922</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C107" s="12">
-        <v>430492</v>
+        <v>399224</v>
       </c>
       <c r="D107" s="9">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="E107" s="9">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="F107" s="9">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="G107" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H107" s="9">
         <f>SUM(D107+F107+G107)</f>
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="I107" s="9">
         <f>H107-E107-F107-G107</f>
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="J107" s="13"/>
       <c r="K107" s="14"/>
@@ -4951,33 +4898,33 @@
     </row>
     <row r="108" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="11">
-        <v>43917</v>
+        <v>43923</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C108" s="12">
-        <v>430492</v>
+        <v>399224</v>
       </c>
       <c r="D108" s="9">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="E108" s="9">
+        <v>36</v>
+      </c>
+      <c r="F108" s="9">
         <v>24</v>
       </c>
-      <c r="F108" s="9">
-        <v>0</v>
-      </c>
       <c r="G108" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H108" s="9">
         <f>SUM(D108+F108+G108)</f>
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="I108" s="9">
         <f>H108-E108-F108-G108</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J108" s="13"/>
       <c r="K108" s="14"/>
@@ -4989,33 +4936,33 @@
     </row>
     <row r="109" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="11">
-        <v>43918</v>
+        <v>43924</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C109" s="12">
-        <v>430492</v>
+        <v>399224</v>
       </c>
       <c r="D109" s="9">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="E109" s="9">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F109" s="9">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G109" s="9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H109" s="9">
         <f>SUM(D109+F109+G109)</f>
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="I109" s="9">
         <f>H109-E109-F109-G109</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J109" s="13"/>
       <c r="K109" s="14"/>
@@ -5027,33 +4974,33 @@
     </row>
     <row r="110" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="11">
-        <v>43919</v>
+        <v>43925</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C110" s="12">
-        <v>430492</v>
+        <v>399224</v>
       </c>
       <c r="D110" s="9">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E110" s="9">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F110" s="9">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G110" s="9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H110" s="9">
         <f>SUM(D110+F110+G110)</f>
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="I110" s="9">
         <f>H110-E110-F110-G110</f>
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="J110" s="13"/>
       <c r="K110" s="14"/>
@@ -5065,33 +5012,33 @@
     </row>
     <row r="111" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="11">
-        <v>43920</v>
+        <v>43926</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C111" s="12">
-        <v>430492</v>
+        <v>399224</v>
       </c>
       <c r="D111" s="9">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E111" s="9">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F111" s="9">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G111" s="9">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H111" s="9">
         <f>SUM(D111+F111+G111)</f>
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="I111" s="9">
         <f>H111-E111-F111-G111</f>
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="J111" s="13"/>
       <c r="K111" s="14"/>
@@ -5103,33 +5050,33 @@
     </row>
     <row r="112" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="11">
-        <v>43921</v>
+        <v>43927</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C112" s="12">
-        <v>430492</v>
+        <v>399224</v>
       </c>
       <c r="D112" s="9">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E112" s="9">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="F112" s="9">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G112" s="9">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="H112" s="9">
         <f>SUM(D112+F112+G112)</f>
-        <v>73</v>
+        <v>111</v>
       </c>
       <c r="I112" s="9">
         <f>H112-E112-F112-G112</f>
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="J112" s="13"/>
       <c r="K112" s="14"/>
@@ -5139,47 +5086,40 @@
       <c r="O112" s="14"/>
       <c r="P112" s="14"/>
     </row>
-    <row r="113" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="11">
-        <v>43922</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>16</v>
+        <v>43928</v>
+      </c>
+      <c r="B113" t="s">
+        <v>15</v>
       </c>
       <c r="C113" s="12">
-        <v>430492</v>
-      </c>
-      <c r="D113" s="9">
-        <v>73</v>
-      </c>
-      <c r="E113" s="9">
-        <v>25</v>
-      </c>
-      <c r="F113" s="9">
-        <v>0</v>
-      </c>
-      <c r="G113" s="9">
-        <v>2</v>
-      </c>
-      <c r="H113" s="9">
+        <v>399224</v>
+      </c>
+      <c r="D113" s="5">
+        <v>80</v>
+      </c>
+      <c r="E113" s="5">
+        <v>42</v>
+      </c>
+      <c r="F113" s="5">
+        <v>26</v>
+      </c>
+      <c r="G113" s="5">
+        <v>7</v>
+      </c>
+      <c r="H113" s="5">
         <f>SUM(D113+F113+G113)</f>
-        <v>75</v>
-      </c>
-      <c r="I113" s="9">
+        <v>113</v>
+      </c>
+      <c r="I113" s="5">
         <f>H113-E113-F113-G113</f>
-        <v>48</v>
-      </c>
-      <c r="J113" s="13"/>
-      <c r="K113" s="14"/>
-      <c r="L113" s="14"/>
-      <c r="M113" s="14"/>
-      <c r="N113" s="14"/>
-      <c r="O113" s="14"/>
-      <c r="P113" s="14"/>
-    </row>
-    <row r="114" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="11">
-        <v>43923</v>
+        <v>43915</v>
       </c>
       <c r="B114" s="8" t="s">
         <v>16</v>
@@ -5188,36 +5128,40 @@
         <v>430492</v>
       </c>
       <c r="D114" s="9">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="E114" s="9">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F114" s="9">
         <v>0</v>
       </c>
       <c r="G114" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H114" s="9">
         <f>SUM(D114+F114+G114)</f>
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="I114" s="9">
         <f>H114-E114-F114-G114</f>
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="J114" s="13"/>
       <c r="K114" s="14"/>
       <c r="L114" s="14"/>
-      <c r="M114" s="14"/>
-      <c r="N114" s="14"/>
-      <c r="O114" s="14"/>
-      <c r="P114" s="14"/>
-    </row>
-    <row r="115" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="M114" s="15"/>
+      <c r="N114" s="12"/>
+      <c r="O114" s="15"/>
+      <c r="P114" s="15"/>
+      <c r="Q114" s="15"/>
+      <c r="R114" s="15"/>
+      <c r="S114" s="15"/>
+      <c r="T114" s="15"/>
+    </row>
+    <row r="115" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="11">
-        <v>43924</v>
+        <v>43916</v>
       </c>
       <c r="B115" s="8" t="s">
         <v>16</v>
@@ -5226,24 +5170,24 @@
         <v>430492</v>
       </c>
       <c r="D115" s="9">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="E115" s="9">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F115" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G115" s="9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H115" s="9">
         <f>SUM(D115+F115+G115)</f>
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="I115" s="9">
         <f>H115-E115-F115-G115</f>
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="J115" s="13"/>
       <c r="K115" s="14"/>
@@ -5253,9 +5197,9 @@
       <c r="O115" s="14"/>
       <c r="P115" s="14"/>
     </row>
-    <row r="116" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="11">
-        <v>43925</v>
+        <v>43917</v>
       </c>
       <c r="B116" s="8" t="s">
         <v>16</v>
@@ -5264,24 +5208,24 @@
         <v>430492</v>
       </c>
       <c r="D116" s="9">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="E116" s="9">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F116" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G116" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H116" s="9">
         <f>SUM(D116+F116+G116)</f>
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="I116" s="9">
         <f>H116-E116-F116-G116</f>
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="J116" s="13"/>
       <c r="K116" s="14"/>
@@ -5291,9 +5235,9 @@
       <c r="O116" s="14"/>
       <c r="P116" s="14"/>
     </row>
-    <row r="117" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="11">
-        <v>43926</v>
+        <v>43918</v>
       </c>
       <c r="B117" s="8" t="s">
         <v>16</v>
@@ -5302,24 +5246,24 @@
         <v>430492</v>
       </c>
       <c r="D117" s="9">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="E117" s="9">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F117" s="9">
+        <v>0</v>
+      </c>
+      <c r="G117" s="9">
         <v>1</v>
-      </c>
-      <c r="G117" s="9">
-        <v>3</v>
       </c>
       <c r="H117" s="9">
         <f>SUM(D117+F117+G117)</f>
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="I117" s="9">
         <f>H117-E117-F117-G117</f>
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="J117" s="13"/>
       <c r="K117" s="14"/>
@@ -5329,9 +5273,9 @@
       <c r="O117" s="14"/>
       <c r="P117" s="14"/>
     </row>
-    <row r="118" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="11">
-        <v>43927</v>
+        <v>43919</v>
       </c>
       <c r="B118" s="8" t="s">
         <v>16</v>
@@ -5340,24 +5284,24 @@
         <v>430492</v>
       </c>
       <c r="D118" s="9">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E118" s="9">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F118" s="9">
+        <v>0</v>
+      </c>
+      <c r="G118" s="9">
         <v>1</v>
-      </c>
-      <c r="G118" s="9">
-        <v>3</v>
       </c>
       <c r="H118" s="9">
         <f>SUM(D118+F118+G118)</f>
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="I118" s="9">
         <f>H118-E118-F118-G118</f>
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="J118" s="13"/>
       <c r="K118" s="14"/>
@@ -5367,10 +5311,345 @@
       <c r="O118" s="14"/>
       <c r="P118" s="14"/>
     </row>
+    <row r="119" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A119" s="11">
+        <v>43920</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C119" s="12">
+        <v>430492</v>
+      </c>
+      <c r="D119" s="9">
+        <v>70</v>
+      </c>
+      <c r="E119" s="9">
+        <v>26</v>
+      </c>
+      <c r="F119" s="9">
+        <v>0</v>
+      </c>
+      <c r="G119" s="9">
+        <v>1</v>
+      </c>
+      <c r="H119" s="9">
+        <f>SUM(D119+F119+G119)</f>
+        <v>71</v>
+      </c>
+      <c r="I119" s="9">
+        <f>H119-E119-F119-G119</f>
+        <v>44</v>
+      </c>
+      <c r="J119" s="13"/>
+      <c r="K119" s="14"/>
+      <c r="L119" s="14"/>
+      <c r="M119" s="14"/>
+      <c r="N119" s="14"/>
+      <c r="O119" s="14"/>
+      <c r="P119" s="14"/>
+    </row>
+    <row r="120" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A120" s="11">
+        <v>43921</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C120" s="12">
+        <v>430492</v>
+      </c>
+      <c r="D120" s="9">
+        <v>72</v>
+      </c>
+      <c r="E120" s="9">
+        <v>26</v>
+      </c>
+      <c r="F120" s="9">
+        <v>0</v>
+      </c>
+      <c r="G120" s="9">
+        <v>1</v>
+      </c>
+      <c r="H120" s="9">
+        <f>SUM(D120+F120+G120)</f>
+        <v>73</v>
+      </c>
+      <c r="I120" s="9">
+        <f>H120-E120-F120-G120</f>
+        <v>46</v>
+      </c>
+      <c r="J120" s="13"/>
+      <c r="K120" s="14"/>
+      <c r="L120" s="14"/>
+      <c r="M120" s="14"/>
+      <c r="N120" s="14"/>
+      <c r="O120" s="14"/>
+      <c r="P120" s="14"/>
+    </row>
+    <row r="121" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A121" s="11">
+        <v>43922</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C121" s="12">
+        <v>430492</v>
+      </c>
+      <c r="D121" s="9">
+        <v>73</v>
+      </c>
+      <c r="E121" s="9">
+        <v>25</v>
+      </c>
+      <c r="F121" s="9">
+        <v>0</v>
+      </c>
+      <c r="G121" s="9">
+        <v>2</v>
+      </c>
+      <c r="H121" s="9">
+        <f>SUM(D121+F121+G121)</f>
+        <v>75</v>
+      </c>
+      <c r="I121" s="9">
+        <f>H121-E121-F121-G121</f>
+        <v>48</v>
+      </c>
+      <c r="J121" s="13"/>
+      <c r="K121" s="14"/>
+      <c r="L121" s="14"/>
+      <c r="M121" s="14"/>
+      <c r="N121" s="14"/>
+      <c r="O121" s="14"/>
+      <c r="P121" s="14"/>
+    </row>
+    <row r="122" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A122" s="11">
+        <v>43923</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C122" s="12">
+        <v>430492</v>
+      </c>
+      <c r="D122" s="9">
+        <v>78</v>
+      </c>
+      <c r="E122" s="9">
+        <v>25</v>
+      </c>
+      <c r="F122" s="9">
+        <v>0</v>
+      </c>
+      <c r="G122" s="9">
+        <v>2</v>
+      </c>
+      <c r="H122" s="9">
+        <f>SUM(D122+F122+G122)</f>
+        <v>80</v>
+      </c>
+      <c r="I122" s="9">
+        <f>H122-E122-F122-G122</f>
+        <v>53</v>
+      </c>
+      <c r="J122" s="13"/>
+      <c r="K122" s="14"/>
+      <c r="L122" s="14"/>
+      <c r="M122" s="14"/>
+      <c r="N122" s="14"/>
+      <c r="O122" s="14"/>
+      <c r="P122" s="14"/>
+    </row>
+    <row r="123" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A123" s="11">
+        <v>43924</v>
+      </c>
+      <c r="B123" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C123" s="12">
+        <v>430492</v>
+      </c>
+      <c r="D123" s="9">
+        <v>78</v>
+      </c>
+      <c r="E123" s="9">
+        <v>24</v>
+      </c>
+      <c r="F123" s="9">
+        <v>1</v>
+      </c>
+      <c r="G123" s="9">
+        <v>2</v>
+      </c>
+      <c r="H123" s="9">
+        <f>SUM(D123+F123+G123)</f>
+        <v>81</v>
+      </c>
+      <c r="I123" s="9">
+        <f>H123-E123-F123-G123</f>
+        <v>54</v>
+      </c>
+      <c r="J123" s="13"/>
+      <c r="K123" s="14"/>
+      <c r="L123" s="14"/>
+      <c r="M123" s="14"/>
+      <c r="N123" s="14"/>
+      <c r="O123" s="14"/>
+      <c r="P123" s="14"/>
+    </row>
+    <row r="124" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A124" s="11">
+        <v>43925</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C124" s="12">
+        <v>430492</v>
+      </c>
+      <c r="D124" s="9">
+        <v>90</v>
+      </c>
+      <c r="E124" s="9">
+        <v>25</v>
+      </c>
+      <c r="F124" s="9">
+        <v>1</v>
+      </c>
+      <c r="G124" s="9">
+        <v>3</v>
+      </c>
+      <c r="H124" s="9">
+        <f>SUM(D124+F124+G124)</f>
+        <v>94</v>
+      </c>
+      <c r="I124" s="9">
+        <f>H124-E124-F124-G124</f>
+        <v>65</v>
+      </c>
+      <c r="J124" s="13"/>
+      <c r="K124" s="14"/>
+      <c r="L124" s="14"/>
+      <c r="M124" s="14"/>
+      <c r="N124" s="14"/>
+      <c r="O124" s="14"/>
+      <c r="P124" s="14"/>
+    </row>
+    <row r="125" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A125" s="11">
+        <v>43926</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C125" s="12">
+        <v>430492</v>
+      </c>
+      <c r="D125" s="9">
+        <v>94</v>
+      </c>
+      <c r="E125" s="9">
+        <v>24</v>
+      </c>
+      <c r="F125" s="9">
+        <v>1</v>
+      </c>
+      <c r="G125" s="9">
+        <v>3</v>
+      </c>
+      <c r="H125" s="9">
+        <f>SUM(D125+F125+G125)</f>
+        <v>98</v>
+      </c>
+      <c r="I125" s="9">
+        <f>H125-E125-F125-G125</f>
+        <v>70</v>
+      </c>
+      <c r="J125" s="13"/>
+      <c r="K125" s="14"/>
+      <c r="L125" s="14"/>
+      <c r="M125" s="14"/>
+      <c r="N125" s="14"/>
+      <c r="O125" s="14"/>
+      <c r="P125" s="14"/>
+    </row>
+    <row r="126" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A126" s="11">
+        <v>43927</v>
+      </c>
+      <c r="B126" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C126" s="12">
+        <v>430492</v>
+      </c>
+      <c r="D126" s="9">
+        <v>100</v>
+      </c>
+      <c r="E126" s="9">
+        <v>24</v>
+      </c>
+      <c r="F126" s="9">
+        <v>1</v>
+      </c>
+      <c r="G126" s="9">
+        <v>3</v>
+      </c>
+      <c r="H126" s="9">
+        <f>SUM(D126+F126+G126)</f>
+        <v>104</v>
+      </c>
+      <c r="I126" s="9">
+        <f>H126-E126-F126-G126</f>
+        <v>76</v>
+      </c>
+      <c r="J126" s="13"/>
+      <c r="K126" s="14"/>
+      <c r="L126" s="14"/>
+      <c r="M126" s="14"/>
+      <c r="N126" s="14"/>
+      <c r="O126" s="14"/>
+      <c r="P126" s="14"/>
+    </row>
+    <row r="127" spans="1:20" ht="16" x14ac:dyDescent="0.2">
+      <c r="A127" s="11">
+        <v>43928</v>
+      </c>
+      <c r="B127" t="s">
+        <v>16</v>
+      </c>
+      <c r="C127" s="12">
+        <v>430492</v>
+      </c>
+      <c r="D127" s="5">
+        <v>105</v>
+      </c>
+      <c r="E127" s="5">
+        <v>22</v>
+      </c>
+      <c r="F127" s="5">
+        <v>1</v>
+      </c>
+      <c r="G127" s="5">
+        <v>3</v>
+      </c>
+      <c r="H127" s="5">
+        <f>SUM(D127+F127+G127)</f>
+        <v>109</v>
+      </c>
+      <c r="I127" s="5">
+        <f>H127-E127-F127-G127</f>
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:T118">
-    <sortState ref="A2:T118">
-      <sortCondition ref="B1:B118"/>
+    <sortState ref="A2:T127">
+      <sortCondition ref="B1:B127"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>